<commit_message>
sửa lỗi chức năng import mã hàng mới
</commit_message>
<xml_diff>
--- a/DatPhatAcc/Resources/MisaExcelTemplates/Mau_danh_muc_vat_tu_hang_hoa_VND.xlsx
+++ b/DatPhatAcc/Resources/MisaExcelTemplates/Mau_danh_muc_vat_tu_hang_hoa_VND.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb4b639525fd57fd/Máy tính/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ducdo\source\repos\DatPhatAcc\DatPhatAcc\Resources\MisaExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{E3768F99-F8EE-402D-ABC8-209628A3FCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F97F02BD-8D1E-43BC-BD5A-0896A560845E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77183672-A401-4C30-8682-3A3074C4072C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="2070" windowWidth="22515" windowHeight="12990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh mục VTHH" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Mã (*)</t>
   </si>
@@ -107,48 +107,6 @@
   </si>
   <si>
     <t>Cho phép trùng</t>
-  </si>
-  <si>
-    <t>01000001</t>
-  </si>
-  <si>
-    <t>Lê Singo S6 -(5KG/hộp)</t>
-  </si>
-  <si>
-    <t>01000002</t>
-  </si>
-  <si>
-    <t>Kẹo dẻo trong 100g</t>
-  </si>
-  <si>
-    <t>01000003</t>
-  </si>
-  <si>
-    <t>Kẹo Fruit Plus vị dâu 150g 48/T</t>
-  </si>
-  <si>
-    <t>01000004</t>
-  </si>
-  <si>
-    <t>Kẹo Fruit plus vị nho 150g 48T</t>
-  </si>
-  <si>
-    <t>01000005</t>
-  </si>
-  <si>
-    <t>DYNAMITTE Chews Fruity 125g/36</t>
-  </si>
-  <si>
-    <t>01000006</t>
-  </si>
-  <si>
-    <t>Kẹo ABC Roll milk trái cây 250g/20</t>
-  </si>
-  <si>
-    <t>01000007</t>
-  </si>
-  <si>
-    <t>Ống kẹo mút hương hỗn hợp Chupa Chups tết 200g/24</t>
   </si>
 </sst>
 </file>
@@ -315,10 +273,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,7 +626,7 @@
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,60 +738,32 @@
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>